<commit_message>
agraga parametros para password y usuario
</commit_message>
<xml_diff>
--- a/src/test/resources/data/productData.xlsx
+++ b/src/test/resources/data/productData.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\repo\PostulacionQA\src\test\resources\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FC0B04-32FC-4208-A433-AD97F3DF8462}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4965" windowWidth="29040" windowHeight="15840" xr2:uid="{D6E58E95-2A08-4D17-A63E-2DF2D71BE4DF}"/>
+    <workbookView xWindow="20370" yWindow="-4965" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,22 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>nombreProducto</t>
   </si>
   <si>
     <t>mouse</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>jpleal79@gmail.com</t>
+  </si>
+  <si>
+    <t>serrano832</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +83,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -134,7 +151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -186,7 +203,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -380,36 +397,53 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE35438-EBD6-45CA-9CE5-8FFC1726B581}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>